<commit_message>
:loud_sound: only 8 audios left
</commit_message>
<xml_diff>
--- a/Cipher-key-music-text.xlsx
+++ b/Cipher-key-music-text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\OneDrive\Documentos\Signals Project\Fourier-Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1B6918-DED9-47DC-8B40-7C27C8595DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3413E6-06DA-4395-A07E-C08A29CAABB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1D06FA13-21DA-4E25-B74A-0658B95FA3B2}"/>
   </bookViews>
@@ -344,7 +344,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +366,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -419,18 +431,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +777,7 @@
   <dimension ref="A2:AF31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B15"/>
+      <selection activeCell="Y6" sqref="Y6:AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,10 +793,10 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="W4" s="4" t="s">
+      <c r="W4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="X4" s="7"/>
+      <c r="X4" s="10"/>
       <c r="Y4" s="3" t="s">
         <v>93</v>
       </c>
@@ -785,33 +806,36 @@
       <c r="AA4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AD4" s="6" t="s">
+      <c r="AD4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AE4" s="9">
+      <c r="AE4" s="7">
         <v>98</v>
       </c>
-      <c r="AF4" s="9">
+      <c r="AF4" s="7">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
       <c r="M5" s="2" t="str">
         <f t="shared" ref="M5:N5" si="0">IFERROR(VLOOKUP(C5,$W$5:$Y$30,3,FALSE), "")</f>
         <v>F3</v>
@@ -851,104 +875,107 @@
       <c r="W5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X5" s="8">
-        <f>COUNTIF($C$5:$K$28,W5)</f>
+      <c r="X5" s="6">
+        <f t="shared" ref="X5:X30" si="2">COUNTIF($C$5:$K$28,W5)</f>
         <v>13</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="Y5" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="Z5" s="16">
         <v>174</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AA5" s="16">
         <v>174</v>
       </c>
-      <c r="AD5" s="6" t="s">
+      <c r="AD5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AE5" s="9">
+      <c r="AE5" s="7">
         <v>110</v>
       </c>
-      <c r="AF5" s="9">
+      <c r="AF5" s="7">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="M6" s="2" t="str">
-        <f t="shared" ref="M6:M27" si="2">IFERROR(VLOOKUP(C6,$W$5:$Y$30,3,FALSE), "")</f>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="M6" s="15" t="str">
+        <f t="shared" ref="M6:M27" si="3">IFERROR(VLOOKUP(C6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>G4</v>
       </c>
-      <c r="N6" s="2" t="str">
-        <f t="shared" ref="N6:N27" si="3">IFERROR(VLOOKUP(D6,$W$5:$Y$30,3,FALSE), "")</f>
+      <c r="N6" s="15" t="str">
+        <f t="shared" ref="N6:N27" si="4">IFERROR(VLOOKUP(D6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>A5</v>
       </c>
-      <c r="O6" s="2" t="str">
-        <f t="shared" ref="O6:O27" si="4">IFERROR(VLOOKUP(E6,$W$5:$Y$30,3,FALSE), "")</f>
+      <c r="O6" s="15" t="str">
+        <f t="shared" ref="O6:O27" si="5">IFERROR(VLOOKUP(E6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>C4</v>
       </c>
-      <c r="P6" s="2" t="str">
-        <f t="shared" ref="P6:P27" si="5">IFERROR(VLOOKUP(F6,$W$5:$Y$30,3,FALSE), "")</f>
+      <c r="P6" s="15" t="str">
+        <f t="shared" ref="P6:P27" si="6">IFERROR(VLOOKUP(F6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>E4</v>
       </c>
-      <c r="Q6" s="2" t="str">
-        <f t="shared" ref="Q6:Q27" si="6">IFERROR(VLOOKUP(G6,$W$5:$Y$30,3,FALSE), "")</f>
+      <c r="Q6" s="15" t="str">
+        <f t="shared" ref="Q6:Q27" si="7">IFERROR(VLOOKUP(G6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>E5</v>
       </c>
-      <c r="R6" s="2" t="str">
-        <f t="shared" ref="R6:R27" si="7">IFERROR(VLOOKUP(H6,$W$5:$Y$30,3,FALSE), "")</f>
+      <c r="R6" s="15" t="str">
+        <f t="shared" ref="R6:R27" si="8">IFERROR(VLOOKUP(H6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>D4</v>
       </c>
       <c r="S6" s="2" t="str">
-        <f t="shared" ref="S6:S27" si="8">IFERROR(VLOOKUP(I6,$W$5:$Y$30,3,FALSE), "")</f>
+        <f t="shared" ref="S6:S27" si="9">IFERROR(VLOOKUP(I6,$W$5:$Y$30,3,FALSE), "")</f>
         <v/>
       </c>
       <c r="T6" s="2" t="str">
-        <f t="shared" ref="T6:T27" si="9">IFERROR(VLOOKUP(J6,$W$5:$Y$30,3,FALSE), "")</f>
+        <f t="shared" ref="T6:T27" si="10">IFERROR(VLOOKUP(J6,$W$5:$Y$30,3,FALSE), "")</f>
         <v/>
       </c>
       <c r="U6" s="2" t="str">
-        <f t="shared" ref="U6:U27" si="10">IFERROR(VLOOKUP(K6,$W$5:$Y$30,3,FALSE), "")</f>
+        <f t="shared" ref="U6:U27" si="11">IFERROR(VLOOKUP(K6,$W$5:$Y$30,3,FALSE), "")</f>
         <v/>
       </c>
       <c r="W6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X6" s="8">
-        <f>COUNTIF($C$5:$K$28,W6)</f>
+      <c r="X6" s="6">
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="Z6" s="16">
         <v>196</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AA6" s="16">
         <v>196</v>
       </c>
       <c r="AD6" s="3" t="s">
@@ -962,74 +989,77 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="A7">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="M7" s="2" t="str">
-        <f t="shared" si="2"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="M7" s="15" t="str">
+        <f t="shared" si="3"/>
         <v>A4</v>
       </c>
-      <c r="N7" s="2" t="str">
-        <f t="shared" si="3"/>
+      <c r="N7" s="15" t="str">
+        <f t="shared" si="4"/>
         <v>G3</v>
       </c>
-      <c r="O7" s="2" t="str">
-        <f t="shared" si="4"/>
+      <c r="O7" s="15" t="str">
+        <f t="shared" si="5"/>
         <v>C4</v>
       </c>
-      <c r="P7" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q7" s="2" t="str">
+      <c r="P7" s="15" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R7" s="2" t="str">
+      <c r="Q7" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
+      <c r="R7" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="S7" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T7" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U7" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="X7" s="8">
-        <f>COUNTIF($C$5:$K$28,W7)</f>
+      <c r="X7" s="6">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="Y7" s="3" t="s">
+      <c r="Y7" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="Z7" s="16">
         <v>220</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AA7" s="16">
         <v>220</v>
       </c>
       <c r="AD7" s="3" t="s">
@@ -1038,254 +1068,266 @@
       <c r="AE7" s="3">
         <v>146</v>
       </c>
-      <c r="AF7" s="10">
+      <c r="AF7" s="8">
         <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="A8">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="M8" s="2" t="str">
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="M8" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>A3</v>
+      </c>
+      <c r="N8" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>G3</v>
+      </c>
+      <c r="O8" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>G5</v>
+      </c>
+      <c r="P8" s="15" t="str">
+        <f t="shared" si="6"/>
+        <v>D4</v>
+      </c>
+      <c r="Q8" s="15" t="str">
+        <f t="shared" si="7"/>
+        <v>C4</v>
+      </c>
+      <c r="R8" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="S8" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T8" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="U8" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="X8" s="6">
         <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Y8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z8" s="13">
+        <v>261</v>
+      </c>
+      <c r="AA8" s="13">
+        <v>262</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>164</v>
+      </c>
+      <c r="AF8" s="8">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>F3</v>
+      </c>
+      <c r="N9" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>A3</v>
       </c>
-      <c r="N8" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>G3</v>
-      </c>
-      <c r="O8" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>G5</v>
-      </c>
-      <c r="P8" s="2" t="str">
+      <c r="O9" s="2" t="str">
         <f t="shared" si="5"/>
         <v>D4</v>
       </c>
-      <c r="Q8" s="2" t="str">
+      <c r="P9" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>C4</v>
-      </c>
-      <c r="R8" s="2" t="str">
+        <v>D5</v>
+      </c>
+      <c r="Q9" s="2" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S8" s="2" t="str">
+        <v>G4</v>
+      </c>
+      <c r="R9" s="2" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="T8" s="2" t="str">
+        <v>G3</v>
+      </c>
+      <c r="S9" s="2" t="str">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="U8" s="2" t="str">
+        <v>E4</v>
+      </c>
+      <c r="T9" s="2" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X8" s="8">
-        <f>COUNTIF($C$5:$K$28,W8)</f>
-        <v>8</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z8" s="9">
-        <v>261</v>
-      </c>
-      <c r="AA8" s="9">
-        <v>262</v>
-      </c>
-      <c r="AD8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE8" s="3">
-        <v>164</v>
-      </c>
-      <c r="AF8" s="10">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>F3</v>
-      </c>
-      <c r="N9" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>A3</v>
-      </c>
-      <c r="O9" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>D4</v>
-      </c>
-      <c r="P9" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>D5</v>
-      </c>
-      <c r="Q9" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>G4</v>
-      </c>
-      <c r="R9" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>G3</v>
-      </c>
-      <c r="S9" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>E4</v>
-      </c>
-      <c r="T9" s="2" t="str">
-        <f t="shared" si="9"/>
         <v>E5</v>
       </c>
       <c r="U9" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>C4</v>
       </c>
       <c r="W9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="X9" s="8">
-        <f>COUNTIF($C$5:$K$28,W9)</f>
+      <c r="X9" s="6">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Y9" s="6" t="s">
+      <c r="Y9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="Z9" s="9">
+      <c r="Z9" s="13">
         <v>293</v>
       </c>
-      <c r="AA9" s="9">
+      <c r="AA9" s="13">
         <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="A10">
         <v>6</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="M10" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>G5</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E4</v>
       </c>
       <c r="O10" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>F3</v>
       </c>
       <c r="P10" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>A3</v>
       </c>
       <c r="Q10" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R10" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S10" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T10" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U10" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X10" s="8">
-        <f>COUNTIF($C$5:$K$28,W10)</f>
+      <c r="X10" s="6">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="Y10" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="Z10" s="9">
+      <c r="Z10" s="13">
         <v>329</v>
       </c>
-      <c r="AA10" s="9">
+      <c r="AA10" s="13">
         <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1313,575 +1355,599 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="M11" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>A4</v>
+      </c>
+      <c r="N11" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>E4</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>D6</v>
+      </c>
+      <c r="P11" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>F3</v>
+      </c>
+      <c r="Q11" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>D5</v>
+      </c>
+      <c r="R11" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>A3</v>
+      </c>
+      <c r="S11" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>G5</v>
+      </c>
+      <c r="T11" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="U11" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="X11" s="6">
         <f t="shared" si="2"/>
-        <v>A4</v>
-      </c>
-      <c r="N11" s="2" t="str">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z11" s="13">
+        <v>392</v>
+      </c>
+      <c r="AA11" s="13">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="M12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>A3</v>
+      </c>
+      <c r="N12" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>G3</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>G4</v>
+      </c>
+      <c r="P12" s="15" t="str">
+        <f t="shared" si="6"/>
+        <v>C6</v>
+      </c>
+      <c r="Q12" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>D5</v>
+      </c>
+      <c r="R12" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>F3</v>
+      </c>
+      <c r="S12" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T12" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="U12" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X12" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Y12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z12" s="13">
+        <v>440</v>
+      </c>
+      <c r="AA12" s="13">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="M13" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>E6</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>F3</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>D5</v>
+      </c>
+      <c r="P13" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>G3</v>
+      </c>
+      <c r="Q13" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="R13" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="S13" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T13" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="U13" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="X13" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Y13" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z13" s="16">
+        <v>523</v>
+      </c>
+      <c r="AA13" s="16">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="M14" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>C4</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>A5</v>
+      </c>
+      <c r="O14" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>F3</v>
+      </c>
+      <c r="P14" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>A3</v>
+      </c>
+      <c r="Q14" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>D4</v>
+      </c>
+      <c r="R14" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="S14" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T14" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="U14" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X14" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Y14" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z14" s="16">
+        <v>587</v>
+      </c>
+      <c r="AA14" s="16">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="M15" s="2" t="str">
         <f t="shared" si="3"/>
         <v>E4</v>
       </c>
-      <c r="O11" s="2" t="str">
+      <c r="N15" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>D6</v>
-      </c>
-      <c r="P11" s="2" t="str">
+        <v>G6</v>
+      </c>
+      <c r="O15" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>F3</v>
-      </c>
-      <c r="Q11" s="2" t="str">
+        <v>A5</v>
+      </c>
+      <c r="P15" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>D5</v>
-      </c>
-      <c r="R11" s="2" t="str">
+        <v>D4</v>
+      </c>
+      <c r="Q15" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>A3</v>
-      </c>
-      <c r="S11" s="2" t="str">
+        <v>C5</v>
+      </c>
+      <c r="R15" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>G5</v>
-      </c>
-      <c r="T11" s="2" t="str">
+        <v/>
+      </c>
+      <c r="S15" s="2" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="U11" s="2" t="str">
+      <c r="T15" s="2" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="W11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="X11" s="8">
-        <f>COUNTIF($C$5:$K$28,W11)</f>
-        <v>6</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z11" s="9">
-        <v>392</v>
-      </c>
-      <c r="AA11" s="9">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="U15" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X15" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Y15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z15" s="16">
+        <v>659</v>
+      </c>
+      <c r="AA15" s="16">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="M16" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>E5</v>
+      </c>
+      <c r="N16" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>G3</v>
+      </c>
+      <c r="O16" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>G4</v>
+      </c>
+      <c r="P16" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q16" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="R16" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="S16" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T16" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="U16" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="X16" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Y16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z16" s="16">
+        <v>784</v>
+      </c>
+      <c r="AA16" s="16">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="M12" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>A3</v>
-      </c>
-      <c r="N12" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>G3</v>
-      </c>
-      <c r="O12" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>G4</v>
-      </c>
-      <c r="P12" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>C6</v>
-      </c>
-      <c r="Q12" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>D5</v>
-      </c>
-      <c r="R12" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>F3</v>
-      </c>
-      <c r="S12" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="T12" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="U12" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="X12" s="8">
-        <f>COUNTIF($C$5:$K$28,W12)</f>
-        <v>5</v>
-      </c>
-      <c r="Y12" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z12" s="9">
-        <v>440</v>
-      </c>
-      <c r="AA12" s="9">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="M13" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>E6</v>
-      </c>
-      <c r="N13" s="2" t="str">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="M17" s="2" t="str">
         <f t="shared" si="3"/>
         <v>F3</v>
       </c>
-      <c r="O13" s="2" t="str">
+      <c r="N17" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>D5</v>
-      </c>
-      <c r="P13" s="2" t="str">
+        <v>A3</v>
+      </c>
+      <c r="O17" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>G3</v>
-      </c>
-      <c r="Q13" s="2" t="str">
+        <v/>
+      </c>
+      <c r="P17" s="2" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R13" s="2" t="str">
+      <c r="Q17" s="2" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="S13" s="2" t="str">
+      <c r="R17" s="2" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="T13" s="2" t="str">
+      <c r="S17" s="2" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="U13" s="2" t="str">
+      <c r="T17" s="2" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="W13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="X13" s="8">
-        <f>COUNTIF($C$5:$K$28,W13)</f>
-        <v>5</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z13" s="3">
-        <v>523</v>
-      </c>
-      <c r="AA13" s="3">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="M14" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>C4</v>
-      </c>
-      <c r="N14" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>A5</v>
-      </c>
-      <c r="O14" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>F3</v>
-      </c>
-      <c r="P14" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>A3</v>
-      </c>
-      <c r="Q14" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>D4</v>
-      </c>
-      <c r="R14" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S14" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="T14" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="U14" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="X14" s="8">
-        <f>COUNTIF($C$5:$K$28,W14)</f>
-        <v>4</v>
-      </c>
-      <c r="Y14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z14" s="3">
-        <v>587</v>
-      </c>
-      <c r="AA14" s="3">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="M15" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>E4</v>
-      </c>
-      <c r="N15" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>G6</v>
-      </c>
-      <c r="O15" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>A5</v>
-      </c>
-      <c r="P15" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>D4</v>
-      </c>
-      <c r="Q15" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>C5</v>
-      </c>
-      <c r="R15" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S15" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="T15" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="U15" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="X15" s="8">
-        <f>COUNTIF($C$5:$K$28,W15)</f>
-        <v>4</v>
-      </c>
-      <c r="Y15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z15" s="3">
-        <v>659</v>
-      </c>
-      <c r="AA15" s="3">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="M16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>E5</v>
-      </c>
-      <c r="N16" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>G3</v>
-      </c>
-      <c r="O16" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>G4</v>
-      </c>
-      <c r="P16" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q16" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R16" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S16" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="T16" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="U16" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="X16" s="8">
-        <f>COUNTIF($C$5:$K$28,W16)</f>
-        <v>4</v>
-      </c>
-      <c r="Y16" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>784</v>
-      </c>
-      <c r="AA16" s="3">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="M17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>F3</v>
-      </c>
-      <c r="N17" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>A3</v>
-      </c>
-      <c r="O17" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P17" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q17" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R17" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="S17" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="T17" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
       <c r="U17" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="X17" s="8">
-        <f>COUNTIF($C$5:$K$28,W17)</f>
+      <c r="X17" s="6">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="Y17" s="3" t="s">
+      <c r="Y17" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="Z17" s="3">
+      <c r="Z17" s="16">
         <v>880</v>
       </c>
-      <c r="AA17" s="3">
+      <c r="AA17" s="16">
         <v>880</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
       <c r="M18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F3</v>
       </c>
       <c r="N18" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>C5</v>
       </c>
       <c r="O18" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="P18" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q18" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R18" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S18" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T18" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U18" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X18" s="8">
-        <f>COUNTIF($C$5:$K$28,W18)</f>
+      <c r="X18" s="6">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="Y18" s="6" t="s">
+      <c r="Y18" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="Z18" s="9">
+      <c r="Z18" s="13">
         <v>1046</v>
       </c>
-      <c r="AA18" s="9">
+      <c r="AA18" s="13">
         <v>1049</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>15</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1903,199 +1969,208 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="M19" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>E5</v>
       </c>
       <c r="N19" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D4</v>
       </c>
       <c r="O19" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C4</v>
       </c>
       <c r="P19" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>G3</v>
       </c>
       <c r="Q19" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R19" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S19" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T19" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U19" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="X19" s="8">
-        <f>COUNTIF($C$5:$K$28,W19)</f>
+      <c r="X19" s="6">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Y19" s="6" t="s">
+      <c r="Y19" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="Z19" s="9">
+      <c r="Z19" s="14">
         <v>1174</v>
       </c>
-      <c r="AA19" s="9">
+      <c r="AA19" s="14">
         <v>1182</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>16</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
       <c r="M20" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>A4</v>
       </c>
       <c r="N20" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F3</v>
       </c>
       <c r="O20" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="P20" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q20" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R20" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S20" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T20" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U20" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="X20" s="8">
-        <f>COUNTIF($C$5:$K$28,W20)</f>
+      <c r="X20" s="6">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Y20" s="6" t="s">
+      <c r="Y20" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="Z20" s="9">
+      <c r="Z20" s="13">
         <v>1318</v>
       </c>
-      <c r="AA20" s="9">
+      <c r="AA20" s="13">
         <v>1324</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>17</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
       <c r="M21" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>G4</v>
       </c>
       <c r="N21" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>E4</v>
       </c>
       <c r="O21" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="P21" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q21" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R21" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S21" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T21" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U21" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="X21" s="8">
-        <f>COUNTIF($C$5:$K$28,W21)</f>
+      <c r="X21" s="6">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Y21" s="6" t="s">
+      <c r="Y21" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="Z21" s="9">
+      <c r="Z21" s="13">
         <v>1567</v>
       </c>
-      <c r="AA21" s="9">
+      <c r="AA21" s="13">
         <v>1573</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>18</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
@@ -2123,59 +2198,62 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="M22" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>C4</v>
       </c>
       <c r="N22" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>G3</v>
       </c>
       <c r="O22" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>G5</v>
       </c>
       <c r="P22" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>F3</v>
       </c>
       <c r="Q22" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>A3</v>
       </c>
       <c r="R22" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>E4</v>
       </c>
       <c r="S22" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>A4</v>
       </c>
       <c r="T22" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U22" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X22" s="8">
-        <f>COUNTIF($C$5:$K$28,W22)</f>
+      <c r="X22" s="6">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Y22" s="6" t="s">
+      <c r="Y22" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="Z22" s="9">
+      <c r="Z22" s="7">
         <v>1760</v>
       </c>
-      <c r="AA22" s="9">
+      <c r="AA22" s="7">
         <v>1773</v>
       </c>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>19</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
@@ -2193,50 +2271,53 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="M23" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>D6</v>
       </c>
       <c r="N23" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>D4</v>
       </c>
       <c r="O23" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="P23" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q23" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R23" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S23" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T23" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U23" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="X23" s="8">
-        <f>COUNTIF($C$5:$K$28,W23)</f>
+      <c r="X23" s="6">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>20</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -2252,113 +2333,119 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="M24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>A6</v>
       </c>
       <c r="N24" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O24" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="P24" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q24" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R24" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S24" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T24" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U24" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="X24" s="8">
-        <f>COUNTIF($C$5:$K$28,W24)</f>
+      <c r="X24" s="6">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>21</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
       <c r="M25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>C4</v>
       </c>
       <c r="N25" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>G3</v>
       </c>
       <c r="O25" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C5</v>
       </c>
       <c r="P25" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q25" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R25" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S25" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T25" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U25" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W25" s="3" t="s">
         <v>62</v>
       </c>
       <c r="X25" s="3">
-        <f>COUNTIF($C$5:$K$28,W25)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>22</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
@@ -2382,50 +2469,53 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="M26" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>A4</v>
       </c>
       <c r="N26" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>G3</v>
       </c>
       <c r="O26" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C6</v>
       </c>
       <c r="P26" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>C5</v>
       </c>
       <c r="Q26" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>F3</v>
       </c>
       <c r="R26" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S26" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T26" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U26" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W26" s="3" t="s">
         <v>63</v>
       </c>
       <c r="X26" s="3">
-        <f>COUNTIF($C$5:$K$28,W26)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>23</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
@@ -2449,81 +2539,81 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="M27" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>C6</v>
       </c>
       <c r="N27" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>F3</v>
       </c>
       <c r="O27" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>G4</v>
       </c>
       <c r="P27" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>G3</v>
       </c>
       <c r="Q27" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>C5</v>
       </c>
       <c r="R27" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="S27" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T27" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="U27" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="W27" s="3" t="s">
         <v>64</v>
       </c>
       <c r="X27" s="3">
-        <f>COUNTIF($C$5:$K$28,W27)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="W28" s="3" t="s">
         <v>65</v>
       </c>
       <c r="X28" s="3">
-        <f>COUNTIF($C$5:$K$28,W28)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="W29" s="3" t="s">
         <v>66</v>
       </c>
       <c r="X29" s="3">
-        <f>COUNTIF($C$5:$K$28,W29)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="W30" s="3" t="s">
         <v>67</v>
       </c>
       <c r="X30" s="3">
-        <f>COUNTIF($C$5:$K$28,W30)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="W31" s="5" t="s">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="W31" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="X31" s="5">
+      <c r="X31" s="4">
         <f>COUNTIF(X5:X30, "&lt;&gt;0")</f>
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
:rocket: audio first version ready
</commit_message>
<xml_diff>
--- a/Cipher-key-music-text.xlsx
+++ b/Cipher-key-music-text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\OneDrive\Documentos\Signals Project\Fourier-Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3413E6-06DA-4395-A07E-C08A29CAABB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1EECC4-1A06-47F9-AC36-967D1118B9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1D06FA13-21DA-4E25-B74A-0658B95FA3B2}"/>
   </bookViews>
@@ -327,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +339,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -436,22 +442,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,7 +781,7 @@
   <dimension ref="A2:AF31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6:AA13"/>
+      <selection activeCell="Y8" sqref="Y8:AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,10 +797,10 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="W4" s="9" t="s">
+      <c r="W4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="X4" s="10"/>
+      <c r="X4" s="14"/>
       <c r="Y4" s="3" t="s">
         <v>93</v>
       </c>
@@ -820,22 +824,22 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
       <c r="M5" s="2" t="str">
         <f t="shared" ref="M5:N5" si="0">IFERROR(VLOOKUP(C5,$W$5:$Y$30,3,FALSE), "")</f>
         <v>F3</v>
@@ -879,13 +883,13 @@
         <f t="shared" ref="X5:X30" si="2">COUNTIF($C$5:$K$28,W5)</f>
         <v>13</v>
       </c>
-      <c r="Y5" s="16" t="s">
+      <c r="Y5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="Z5" s="16">
+      <c r="Z5" s="12">
         <v>174</v>
       </c>
-      <c r="AA5" s="16">
+      <c r="AA5" s="12">
         <v>174</v>
       </c>
       <c r="AD5" s="5" t="s">
@@ -902,51 +906,51 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="M6" s="15" t="str">
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="M6" s="2" t="str">
         <f t="shared" ref="M6:M27" si="3">IFERROR(VLOOKUP(C6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>G4</v>
       </c>
-      <c r="N6" s="15" t="str">
+      <c r="N6" s="2" t="str">
         <f t="shared" ref="N6:N27" si="4">IFERROR(VLOOKUP(D6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>A5</v>
       </c>
-      <c r="O6" s="15" t="str">
+      <c r="O6" s="2" t="str">
         <f t="shared" ref="O6:O27" si="5">IFERROR(VLOOKUP(E6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>C4</v>
       </c>
-      <c r="P6" s="15" t="str">
+      <c r="P6" s="2" t="str">
         <f t="shared" ref="P6:P27" si="6">IFERROR(VLOOKUP(F6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>E4</v>
       </c>
-      <c r="Q6" s="15" t="str">
+      <c r="Q6" s="2" t="str">
         <f t="shared" ref="Q6:Q27" si="7">IFERROR(VLOOKUP(G6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>E5</v>
       </c>
-      <c r="R6" s="15" t="str">
+      <c r="R6" s="2" t="str">
         <f t="shared" ref="R6:R27" si="8">IFERROR(VLOOKUP(H6,$W$5:$Y$30,3,FALSE), "")</f>
         <v>D4</v>
       </c>
@@ -969,13 +973,13 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="Y6" s="16" t="s">
+      <c r="Y6" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="Z6" s="16">
+      <c r="Z6" s="15">
         <v>196</v>
       </c>
-      <c r="AA6" s="16">
+      <c r="AA6" s="15">
         <v>196</v>
       </c>
       <c r="AD6" s="3" t="s">
@@ -992,45 +996,45 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="M7" s="15" t="str">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="M7" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A4</v>
       </c>
-      <c r="N7" s="15" t="str">
+      <c r="N7" s="2" t="str">
         <f t="shared" si="4"/>
         <v>G3</v>
       </c>
-      <c r="O7" s="15" t="str">
+      <c r="O7" s="2" t="str">
         <f t="shared" si="5"/>
         <v>C4</v>
       </c>
-      <c r="P7" s="15" t="str">
+      <c r="P7" s="2" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Q7" s="15" t="str">
+      <c r="Q7" s="2" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="R7" s="15" t="str">
+      <c r="R7" s="2" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1053,13 +1057,13 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="Y7" s="16" t="s">
+      <c r="Y7" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z7" s="16">
+      <c r="Z7" s="15">
         <v>220</v>
       </c>
-      <c r="AA7" s="16">
+      <c r="AA7" s="15">
         <v>220</v>
       </c>
       <c r="AD7" s="3" t="s">
@@ -1076,49 +1080,49 @@
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="M8" s="15" t="str">
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="M8" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A3</v>
       </c>
-      <c r="N8" s="15" t="str">
+      <c r="N8" s="2" t="str">
         <f t="shared" si="4"/>
         <v>G3</v>
       </c>
-      <c r="O8" s="15" t="str">
+      <c r="O8" s="2" t="str">
         <f t="shared" si="5"/>
         <v>G5</v>
       </c>
-      <c r="P8" s="15" t="str">
+      <c r="P8" s="2" t="str">
         <f t="shared" si="6"/>
         <v>D4</v>
       </c>
-      <c r="Q8" s="15" t="str">
+      <c r="Q8" s="2" t="str">
         <f t="shared" si="7"/>
         <v>C4</v>
       </c>
-      <c r="R8" s="15" t="str">
+      <c r="R8" s="2" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1141,13 +1145,13 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Y8" s="13" t="s">
+      <c r="Y8" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="Z8" s="16">
         <v>261</v>
       </c>
-      <c r="AA8" s="13">
+      <c r="AA8" s="16">
         <v>262</v>
       </c>
       <c r="AD8" s="3" t="s">
@@ -1164,34 +1168,34 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="10" t="s">
         <v>42</v>
       </c>
       <c r="M9" s="2" t="str">
@@ -1237,13 +1241,13 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Y9" s="13" t="s">
+      <c r="Y9" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="Z9" s="13">
+      <c r="Z9" s="16">
         <v>293</v>
       </c>
-      <c r="AA9" s="13">
+      <c r="AA9" s="16">
         <v>293</v>
       </c>
     </row>
@@ -1251,26 +1255,26 @@
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
       <c r="M10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>G5</v>
@@ -1314,13 +1318,13 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Y10" s="13" t="s">
+      <c r="Y10" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="Z10" s="16">
         <v>329</v>
       </c>
-      <c r="AA10" s="13">
+      <c r="AA10" s="16">
         <v>330</v>
       </c>
     </row>
@@ -1328,32 +1332,32 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
       <c r="M11" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A4</v>
@@ -1397,13 +1401,13 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="Y11" s="13" t="s">
+      <c r="Y11" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="Z11" s="13">
+      <c r="Z11" s="16">
         <v>392</v>
       </c>
-      <c r="AA11" s="13">
+      <c r="AA11" s="16">
         <v>392</v>
       </c>
     </row>
@@ -1411,30 +1415,30 @@
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
       <c r="M12" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A3</v>
@@ -1447,7 +1451,7 @@
         <f t="shared" si="5"/>
         <v>G4</v>
       </c>
-      <c r="P12" s="15" t="str">
+      <c r="P12" s="2" t="str">
         <f t="shared" si="6"/>
         <v>C6</v>
       </c>
@@ -1478,13 +1482,13 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="Y12" s="13" t="s">
+      <c r="Y12" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="Z12" s="13">
+      <c r="Z12" s="16">
         <v>440</v>
       </c>
-      <c r="AA12" s="13">
+      <c r="AA12" s="16">
         <v>440</v>
       </c>
     </row>
@@ -1492,26 +1496,26 @@
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
       <c r="M13" s="2" t="str">
         <f t="shared" si="3"/>
         <v>E6</v>
@@ -1555,13 +1559,13 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="Y13" s="16" t="s">
+      <c r="Y13" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Z13" s="16">
+      <c r="Z13" s="11">
         <v>523</v>
       </c>
-      <c r="AA13" s="16">
+      <c r="AA13" s="11">
         <v>523</v>
       </c>
     </row>
@@ -1569,28 +1573,28 @@
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
       <c r="M14" s="2" t="str">
         <f t="shared" si="3"/>
         <v>C4</v>
@@ -1599,7 +1603,7 @@
         <f t="shared" si="4"/>
         <v>A5</v>
       </c>
-      <c r="O14" s="15" t="str">
+      <c r="O14" s="2" t="str">
         <f t="shared" si="5"/>
         <v>F3</v>
       </c>
@@ -1634,13 +1638,13 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Y14" s="16" t="s">
+      <c r="Y14" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="Z14" s="16">
+      <c r="Z14" s="11">
         <v>587</v>
       </c>
-      <c r="AA14" s="16">
+      <c r="AA14" s="11">
         <v>587</v>
       </c>
     </row>
@@ -1648,28 +1652,28 @@
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
       <c r="M15" s="2" t="str">
         <f t="shared" si="3"/>
         <v>E4</v>
@@ -1686,7 +1690,7 @@
         <f t="shared" si="6"/>
         <v>D4</v>
       </c>
-      <c r="Q15" s="15" t="str">
+      <c r="Q15" s="2" t="str">
         <f t="shared" si="7"/>
         <v>C5</v>
       </c>
@@ -1713,13 +1717,13 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Y15" s="16" t="s">
+      <c r="Y15" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="Z15" s="16">
+      <c r="Z15" s="11">
         <v>659</v>
       </c>
-      <c r="AA15" s="16">
+      <c r="AA15" s="11">
         <v>660</v>
       </c>
     </row>
@@ -1727,24 +1731,24 @@
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
       <c r="M16" s="2" t="str">
         <f t="shared" si="3"/>
         <v>E5</v>
@@ -1788,13 +1792,13 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Y16" s="16" t="s">
+      <c r="Y16" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="Z16" s="16">
+      <c r="Z16" s="12">
         <v>784</v>
       </c>
-      <c r="AA16" s="16">
+      <c r="AA16" s="12">
         <v>784</v>
       </c>
     </row>
@@ -1802,22 +1806,22 @@
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
       <c r="M17" s="2" t="str">
         <f t="shared" si="3"/>
         <v>F3</v>
@@ -1861,13 +1865,13 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="Y17" s="16" t="s">
+      <c r="Y17" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="Z17" s="16">
+      <c r="Z17" s="11">
         <v>880</v>
       </c>
-      <c r="AA17" s="16">
+      <c r="AA17" s="11">
         <v>880</v>
       </c>
     </row>
@@ -1875,22 +1879,22 @@
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
       <c r="M18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>F3</v>
@@ -1934,13 +1938,13 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="Y18" s="13" t="s">
+      <c r="Y18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="Z18" s="13">
+      <c r="Z18" s="5">
         <v>1046</v>
       </c>
-      <c r="AA18" s="13">
+      <c r="AA18" s="5">
         <v>1049</v>
       </c>
     </row>
@@ -1948,26 +1952,26 @@
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
       <c r="M19" s="2" t="str">
         <f t="shared" si="3"/>
         <v>E5</v>
@@ -2011,13 +2015,13 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="Y19" s="13" t="s">
+      <c r="Y19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="Z19" s="14">
+      <c r="Z19" s="5">
         <v>1174</v>
       </c>
-      <c r="AA19" s="14">
+      <c r="AA19" s="5">
         <v>1182</v>
       </c>
     </row>
@@ -2025,22 +2029,22 @@
       <c r="A20">
         <v>16</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
       <c r="M20" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A4</v>
@@ -2084,13 +2088,13 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Y20" s="13" t="s">
+      <c r="Y20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="Z20" s="13">
+      <c r="Z20" s="5">
         <v>1318</v>
       </c>
-      <c r="AA20" s="13">
+      <c r="AA20" s="5">
         <v>1324</v>
       </c>
     </row>
@@ -2098,22 +2102,22 @@
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
       <c r="M21" s="2" t="str">
         <f t="shared" si="3"/>
         <v>G4</v>
@@ -2157,13 +2161,13 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Y21" s="13" t="s">
+      <c r="Y21" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="Z21" s="13">
+      <c r="Z21" s="5">
         <v>1567</v>
       </c>
-      <c r="AA21" s="13">
+      <c r="AA21" s="5">
         <v>1573</v>
       </c>
     </row>
@@ -2171,32 +2175,32 @@
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
       <c r="M22" s="2" t="str">
         <f t="shared" si="3"/>
         <v>C4</v>
@@ -2243,10 +2247,10 @@
       <c r="Y22" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="Z22" s="7">
+      <c r="Z22" s="5">
         <v>1760</v>
       </c>
-      <c r="AA22" s="7">
+      <c r="AA22" s="5">
         <v>1773</v>
       </c>
     </row>
@@ -2254,22 +2258,22 @@
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
       <c r="M23" s="2" t="str">
         <f t="shared" si="3"/>
         <v>D6</v>
@@ -2318,20 +2322,20 @@
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
       <c r="M24" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A6</v>
@@ -2380,24 +2384,24 @@
       <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
       <c r="M25" s="2" t="str">
         <f t="shared" si="3"/>
         <v>C4</v>
@@ -2446,28 +2450,28 @@
       <c r="A26">
         <v>22</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
       <c r="M26" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A4</v>
@@ -2516,28 +2520,28 @@
       <c r="A27">
         <v>23</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
       <c r="M27" s="2" t="str">
         <f t="shared" si="3"/>
         <v>C6</v>

</xml_diff>

<commit_message>
:rocket: audio v2, includes letter repetition >0.2
</commit_message>
<xml_diff>
--- a/Cipher-key-music-text.xlsx
+++ b/Cipher-key-music-text.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\OneDrive\Documentos\Signals Project\Fourier-Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1EECC4-1A06-47F9-AC36-967D1118B9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745682F1-E4F9-42E8-8E66-483AC534762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1D06FA13-21DA-4E25-B74A-0658B95FA3B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{1D06FA13-21DA-4E25-B74A-0658B95FA3B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="95">
   <si>
     <t>En música, dos notas enarmónicas tienen diferente nombre pero suenan igual. Como en el caso de Mi sostenido, Fa, y Sol doble bemol</t>
   </si>
@@ -327,7 +328,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +345,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -428,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,20 +462,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -780,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB32B4B-C86F-4B30-8506-CEF18F4A6E96}">
   <dimension ref="A2:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8:AA12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,10 +829,10 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="W4" s="13" t="s">
+      <c r="W4" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="X4" s="14"/>
+      <c r="X4" s="19"/>
       <c r="Y4" s="3" t="s">
         <v>93</v>
       </c>
@@ -821,10 +853,10 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="21">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -883,13 +915,13 @@
         <f t="shared" ref="X5:X30" si="2">COUNTIF($C$5:$K$28,W5)</f>
         <v>13</v>
       </c>
-      <c r="Y5" s="12" t="s">
+      <c r="Y5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="Z5" s="12">
+      <c r="Z5" s="11">
         <v>174</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AA5" s="11">
         <v>174</v>
       </c>
       <c r="AD5" s="5" t="s">
@@ -903,10 +935,10 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="21">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -973,13 +1005,13 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="Y6" s="15" t="s">
+      <c r="Y6" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="Z6" s="15">
+      <c r="Z6" s="11">
         <v>196</v>
       </c>
-      <c r="AA6" s="15">
+      <c r="AA6" s="11">
         <v>196</v>
       </c>
       <c r="AD6" s="3" t="s">
@@ -993,10 +1025,10 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="21">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1057,13 +1089,13 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="Y7" s="15" t="s">
+      <c r="Y7" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="Z7" s="15">
+      <c r="Z7" s="14">
         <v>220</v>
       </c>
-      <c r="AA7" s="15">
+      <c r="AA7" s="14">
         <v>220</v>
       </c>
       <c r="AD7" s="3" t="s">
@@ -1077,10 +1109,10 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="21">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1145,13 +1177,13 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="Y8" s="16" t="s">
+      <c r="Y8" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="Z8" s="16">
+      <c r="Z8" s="13">
         <v>261</v>
       </c>
-      <c r="AA8" s="16">
+      <c r="AA8" s="13">
         <v>262</v>
       </c>
       <c r="AD8" s="3" t="s">
@@ -1165,10 +1197,10 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="21">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1202,11 +1234,11 @@
         <f t="shared" si="3"/>
         <v>F3</v>
       </c>
-      <c r="N9" s="2" t="str">
+      <c r="N9" s="12" t="str">
         <f t="shared" si="4"/>
         <v>A3</v>
       </c>
-      <c r="O9" s="2" t="str">
+      <c r="O9" s="12" t="str">
         <f t="shared" si="5"/>
         <v>D4</v>
       </c>
@@ -1241,40 +1273,40 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Y9" s="16" t="s">
+      <c r="Y9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="Z9" s="16">
+      <c r="Z9" s="13">
         <v>293</v>
       </c>
-      <c r="AA9" s="16">
+      <c r="AA9" s="13">
         <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="21">
         <v>6</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="M10" s="2" t="str">
         <f t="shared" si="3"/>
         <v>G5</v>
@@ -1283,11 +1315,11 @@
         <f t="shared" si="4"/>
         <v>E4</v>
       </c>
-      <c r="O10" s="2" t="str">
+      <c r="O10" s="12" t="str">
         <f t="shared" si="5"/>
         <v>F3</v>
       </c>
-      <c r="P10" s="2" t="str">
+      <c r="P10" s="12" t="str">
         <f t="shared" si="6"/>
         <v>A3</v>
       </c>
@@ -1318,21 +1350,21 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Y10" s="16" t="s">
+      <c r="Y10" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="Z10" s="16">
+      <c r="Z10" s="15">
         <v>329</v>
       </c>
-      <c r="AA10" s="16">
+      <c r="AA10" s="15">
         <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="21">
         <v>7</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1370,7 +1402,7 @@
         <f t="shared" si="5"/>
         <v>D6</v>
       </c>
-      <c r="P11" s="2" t="str">
+      <c r="P11" s="12" t="str">
         <f t="shared" si="6"/>
         <v>F3</v>
       </c>
@@ -1401,21 +1433,21 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="Y11" s="16" t="s">
+      <c r="Y11" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="Z11" s="16">
+      <c r="Z11" s="13">
         <v>392</v>
       </c>
-      <c r="AA11" s="16">
+      <c r="AA11" s="13">
         <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="21">
         <v>8</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1482,21 +1514,21 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="Y12" s="16" t="s">
+      <c r="Y12" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="Z12" s="16">
+      <c r="Z12" s="13">
         <v>440</v>
       </c>
-      <c r="AA12" s="16">
+      <c r="AA12" s="13">
         <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="21">
         <v>9</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1570,10 +1602,10 @@
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="21">
         <v>10</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1607,7 +1639,7 @@
         <f t="shared" si="5"/>
         <v>F3</v>
       </c>
-      <c r="P14" s="2" t="str">
+      <c r="P14" s="12" t="str">
         <f t="shared" si="6"/>
         <v>A3</v>
       </c>
@@ -1649,10 +1681,10 @@
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="21">
         <v>11</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1728,10 +1760,10 @@
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="21">
         <v>12</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1753,7 +1785,7 @@
         <f t="shared" si="3"/>
         <v>E5</v>
       </c>
-      <c r="N16" s="2" t="str">
+      <c r="N16" s="12" t="str">
         <f t="shared" si="4"/>
         <v>G3</v>
       </c>
@@ -1792,21 +1824,21 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="Y16" s="12" t="s">
+      <c r="Y16" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="Z16" s="12">
+      <c r="Z16" s="14">
         <v>784</v>
       </c>
-      <c r="AA16" s="12">
+      <c r="AA16" s="14">
         <v>784</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="21">
         <v>13</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1876,10 +1908,10 @@
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="21">
         <v>14</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1949,10 +1981,10 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="21">
         <v>15</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -2026,10 +2058,10 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="21">
         <v>16</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -2099,10 +2131,10 @@
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="21">
         <v>17</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -2172,10 +2204,10 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="21">
         <v>18</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -2201,11 +2233,11 @@
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
-      <c r="M22" s="2" t="str">
+      <c r="M22" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C4</v>
       </c>
-      <c r="N22" s="2" t="str">
+      <c r="N22" s="12" t="str">
         <f t="shared" si="4"/>
         <v>G3</v>
       </c>
@@ -2244,21 +2276,21 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Y22" s="5" t="s">
+      <c r="Y22" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="Z22" s="5">
+      <c r="Z22" s="16">
         <v>1760</v>
       </c>
-      <c r="AA22" s="5">
+      <c r="AA22" s="16">
         <v>1773</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="21">
         <v>19</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -2319,10 +2351,10 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="21">
         <v>20</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -2381,10 +2413,10 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="21">
         <v>21</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="20" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -2447,10 +2479,10 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="21">
         <v>22</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -2517,10 +2549,10 @@
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="21">
         <v>23</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -2630,7 +2662,7 @@
     <mergeCell ref="W4:X4"/>
   </mergeCells>
   <conditionalFormatting sqref="W5:W31">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>"IF($W$2:$W$27&lt;&gt;"""")"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2647,5 +2679,2754 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8CF093-7BA6-4B9D-9E3D-86BEDD90B65B}">
+  <dimension ref="A2:AP31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="11" width="3.88671875" style="1" customWidth="1"/>
+    <col min="13" max="21" width="3.88671875" style="1" customWidth="1"/>
+    <col min="23" max="28" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="4" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AG4" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO4" s="7">
+        <v>98</v>
+      </c>
+      <c r="AP4" s="7">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="10" t="str">
+        <f t="shared" ref="M5:M20" si="0">IFERROR(VLOOKUP(C5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v>A6</v>
+      </c>
+      <c r="N5" s="10" t="str">
+        <f t="shared" ref="N5:N20" si="1">IFERROR(VLOOKUP(D5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v>A3</v>
+      </c>
+      <c r="O5" s="10" t="str">
+        <f t="shared" ref="O5:O20" si="2">IFERROR(VLOOKUP(E5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="P5" s="10" t="str">
+        <f t="shared" ref="P5:P20" si="3">IFERROR(VLOOKUP(F5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="10" t="str">
+        <f t="shared" ref="Q5:Q20" si="4">IFERROR(VLOOKUP(G5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="R5" s="10" t="str">
+        <f t="shared" ref="R5:R20" si="5">IFERROR(VLOOKUP(H5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S5" s="10" t="str">
+        <f t="shared" ref="S5:S20" si="6">IFERROR(VLOOKUP(I5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T5" s="10" t="str">
+        <f t="shared" ref="T5:T20" si="7">IFERROR(VLOOKUP(J5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U5" s="10" t="str">
+        <f t="shared" ref="U5:U20" si="8">IFERROR(VLOOKUP(K5,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V5" s="17"/>
+      <c r="W5" s="10">
+        <f>IFERROR(VLOOKUP(C5,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v>1760</v>
+      </c>
+      <c r="X5" s="10">
+        <f t="shared" ref="X5:AE20" si="9">IFERROR(VLOOKUP(D5,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v>220</v>
+      </c>
+      <c r="Y5" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Z5" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA5" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB5" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC5" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD5" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE5" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH5" s="6">
+        <f t="shared" ref="AH5:AH30" si="10">COUNTIF($C$5:$K$28,AG5)</f>
+        <v>13</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>1760</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>1773</v>
+      </c>
+      <c r="AN5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO5" s="7">
+        <v>110</v>
+      </c>
+      <c r="AP5" s="7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>G4</v>
+      </c>
+      <c r="N6" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>A5</v>
+      </c>
+      <c r="O6" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>C4</v>
+      </c>
+      <c r="P6" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>G3</v>
+      </c>
+      <c r="Q6" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>E5</v>
+      </c>
+      <c r="R6" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>D4</v>
+      </c>
+      <c r="S6" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T6" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U6" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V6" s="17"/>
+      <c r="W6" s="10">
+        <f t="shared" ref="W6:W27" si="11">IFERROR(VLOOKUP(C6,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v>392</v>
+      </c>
+      <c r="X6" s="10">
+        <f t="shared" si="9"/>
+        <v>880</v>
+      </c>
+      <c r="Y6" s="10">
+        <f t="shared" si="9"/>
+        <v>261</v>
+      </c>
+      <c r="Z6" s="10">
+        <f t="shared" si="9"/>
+        <v>196</v>
+      </c>
+      <c r="AA6" s="10">
+        <f t="shared" si="9"/>
+        <v>659</v>
+      </c>
+      <c r="AB6" s="10">
+        <f t="shared" si="9"/>
+        <v>293</v>
+      </c>
+      <c r="AC6" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD6" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE6" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH6" s="6">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="AI6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ6" s="13">
+        <v>329</v>
+      </c>
+      <c r="AK6" s="13">
+        <v>330</v>
+      </c>
+      <c r="AN6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO6" s="3">
+        <v>130</v>
+      </c>
+      <c r="AP6" s="3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A4</v>
+      </c>
+      <c r="N7" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="O7" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>C4</v>
+      </c>
+      <c r="P7" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q7" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R7" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S7" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T7" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U7" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V7" s="17"/>
+      <c r="W7" s="10">
+        <f t="shared" si="11"/>
+        <v>440</v>
+      </c>
+      <c r="X7" s="10">
+        <f t="shared" si="9"/>
+        <v>329</v>
+      </c>
+      <c r="Y7" s="10">
+        <f t="shared" si="9"/>
+        <v>261</v>
+      </c>
+      <c r="Z7" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA7" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB7" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC7" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD7" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE7" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH7" s="6">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="AI7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ7" s="11">
+        <v>220</v>
+      </c>
+      <c r="AK7" s="11">
+        <v>220</v>
+      </c>
+      <c r="AN7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO7" s="3">
+        <v>146</v>
+      </c>
+      <c r="AP7" s="8">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A3</v>
+      </c>
+      <c r="N8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="O8" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>G5</v>
+      </c>
+      <c r="P8" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>D4</v>
+      </c>
+      <c r="Q8" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>C4</v>
+      </c>
+      <c r="R8" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S8" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T8" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U8" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V8" s="17"/>
+      <c r="W8" s="10">
+        <f t="shared" si="11"/>
+        <v>220</v>
+      </c>
+      <c r="X8" s="10">
+        <f t="shared" si="9"/>
+        <v>329</v>
+      </c>
+      <c r="Y8" s="10">
+        <f t="shared" si="9"/>
+        <v>784</v>
+      </c>
+      <c r="Z8" s="10">
+        <f t="shared" si="9"/>
+        <v>293</v>
+      </c>
+      <c r="AA8" s="10">
+        <f t="shared" si="9"/>
+        <v>261</v>
+      </c>
+      <c r="AB8" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC8" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD8" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE8" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH8" s="6">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="AI8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ8" s="13">
+        <v>261</v>
+      </c>
+      <c r="AK8" s="13">
+        <v>262</v>
+      </c>
+      <c r="AN8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO8" s="3">
+        <v>164</v>
+      </c>
+      <c r="AP8" s="8">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A6</v>
+      </c>
+      <c r="N9" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>A3</v>
+      </c>
+      <c r="O9" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>D4</v>
+      </c>
+      <c r="P9" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>D5</v>
+      </c>
+      <c r="Q9" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>G4</v>
+      </c>
+      <c r="R9" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>E4</v>
+      </c>
+      <c r="S9" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>G3</v>
+      </c>
+      <c r="T9" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v>E5</v>
+      </c>
+      <c r="U9" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>C4</v>
+      </c>
+      <c r="V9" s="17"/>
+      <c r="W9" s="10">
+        <f t="shared" si="11"/>
+        <v>1760</v>
+      </c>
+      <c r="X9" s="22">
+        <f t="shared" si="9"/>
+        <v>220</v>
+      </c>
+      <c r="Y9" s="22">
+        <f t="shared" si="9"/>
+        <v>293</v>
+      </c>
+      <c r="Z9" s="10">
+        <f t="shared" si="9"/>
+        <v>587</v>
+      </c>
+      <c r="AA9" s="10">
+        <f t="shared" si="9"/>
+        <v>392</v>
+      </c>
+      <c r="AB9" s="10">
+        <f t="shared" si="9"/>
+        <v>329</v>
+      </c>
+      <c r="AC9" s="10">
+        <f t="shared" si="9"/>
+        <v>196</v>
+      </c>
+      <c r="AD9" s="10">
+        <f t="shared" si="9"/>
+        <v>659</v>
+      </c>
+      <c r="AE9" s="10">
+        <f t="shared" si="9"/>
+        <v>261</v>
+      </c>
+      <c r="AG9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH9" s="6">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="AI9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ9" s="13">
+        <v>293</v>
+      </c>
+      <c r="AK9" s="13">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>G5</v>
+      </c>
+      <c r="N10" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>G3</v>
+      </c>
+      <c r="O10" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>A6</v>
+      </c>
+      <c r="P10" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>A3</v>
+      </c>
+      <c r="Q10" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R10" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S10" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T10" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U10" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V10" s="17"/>
+      <c r="W10" s="10">
+        <f t="shared" si="11"/>
+        <v>784</v>
+      </c>
+      <c r="X10" s="10">
+        <f t="shared" si="9"/>
+        <v>196</v>
+      </c>
+      <c r="Y10" s="22">
+        <f t="shared" si="9"/>
+        <v>1760</v>
+      </c>
+      <c r="Z10" s="22">
+        <f t="shared" si="9"/>
+        <v>220</v>
+      </c>
+      <c r="AA10" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB10" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC10" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD10" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE10" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH10" s="6">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="AI10" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ10" s="11">
+        <v>196</v>
+      </c>
+      <c r="AK10" s="11">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A4</v>
+      </c>
+      <c r="N11" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>G3</v>
+      </c>
+      <c r="O11" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>D6</v>
+      </c>
+      <c r="P11" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>A6</v>
+      </c>
+      <c r="Q11" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>D5</v>
+      </c>
+      <c r="R11" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>A3</v>
+      </c>
+      <c r="S11" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>G5</v>
+      </c>
+      <c r="T11" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U11" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V11" s="17"/>
+      <c r="W11" s="10">
+        <f t="shared" si="11"/>
+        <v>440</v>
+      </c>
+      <c r="X11" s="10">
+        <f t="shared" si="9"/>
+        <v>196</v>
+      </c>
+      <c r="Y11" s="10">
+        <f t="shared" si="9"/>
+        <v>1174</v>
+      </c>
+      <c r="Z11" s="22">
+        <f t="shared" si="9"/>
+        <v>1760</v>
+      </c>
+      <c r="AA11" s="10">
+        <f t="shared" si="9"/>
+        <v>587</v>
+      </c>
+      <c r="AB11" s="10">
+        <f t="shared" si="9"/>
+        <v>220</v>
+      </c>
+      <c r="AC11" s="10">
+        <f t="shared" si="9"/>
+        <v>784</v>
+      </c>
+      <c r="AD11" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE11" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH11" s="6">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="AI11" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ11" s="13">
+        <v>392</v>
+      </c>
+      <c r="AK11" s="13">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A3</v>
+      </c>
+      <c r="N12" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="O12" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>G4</v>
+      </c>
+      <c r="P12" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>C6</v>
+      </c>
+      <c r="Q12" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>D5</v>
+      </c>
+      <c r="R12" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>A6</v>
+      </c>
+      <c r="S12" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T12" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U12" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V12" s="17"/>
+      <c r="W12" s="10">
+        <f t="shared" si="11"/>
+        <v>220</v>
+      </c>
+      <c r="X12" s="10">
+        <f t="shared" si="9"/>
+        <v>329</v>
+      </c>
+      <c r="Y12" s="10">
+        <f t="shared" si="9"/>
+        <v>392</v>
+      </c>
+      <c r="Z12" s="10">
+        <f t="shared" si="9"/>
+        <v>1046</v>
+      </c>
+      <c r="AA12" s="10">
+        <f t="shared" si="9"/>
+        <v>587</v>
+      </c>
+      <c r="AB12" s="10">
+        <f t="shared" si="9"/>
+        <v>1760</v>
+      </c>
+      <c r="AC12" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD12" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE12" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH12" s="6">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="AI12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ12" s="13">
+        <v>440</v>
+      </c>
+      <c r="AK12" s="13">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>E6</v>
+      </c>
+      <c r="N13" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>A6</v>
+      </c>
+      <c r="O13" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>D5</v>
+      </c>
+      <c r="P13" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>E4</v>
+      </c>
+      <c r="Q13" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R13" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S13" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T13" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U13" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V13" s="17"/>
+      <c r="W13" s="10">
+        <f t="shared" si="11"/>
+        <v>1318</v>
+      </c>
+      <c r="X13" s="10">
+        <f t="shared" si="9"/>
+        <v>1760</v>
+      </c>
+      <c r="Y13" s="10">
+        <f t="shared" si="9"/>
+        <v>587</v>
+      </c>
+      <c r="Z13" s="10">
+        <f t="shared" si="9"/>
+        <v>329</v>
+      </c>
+      <c r="AA13" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB13" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC13" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD13" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE13" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH13" s="6">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="AI13" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ13" s="11">
+        <v>523</v>
+      </c>
+      <c r="AK13" s="11">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>C4</v>
+      </c>
+      <c r="N14" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>A5</v>
+      </c>
+      <c r="O14" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>A6</v>
+      </c>
+      <c r="P14" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v>A3</v>
+      </c>
+      <c r="Q14" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>D4</v>
+      </c>
+      <c r="R14" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S14" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T14" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U14" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V14" s="17"/>
+      <c r="W14" s="10">
+        <f t="shared" si="11"/>
+        <v>261</v>
+      </c>
+      <c r="X14" s="10">
+        <f t="shared" si="9"/>
+        <v>880</v>
+      </c>
+      <c r="Y14" s="10">
+        <f t="shared" si="9"/>
+        <v>1760</v>
+      </c>
+      <c r="Z14" s="22">
+        <f t="shared" si="9"/>
+        <v>220</v>
+      </c>
+      <c r="AA14" s="10">
+        <f t="shared" si="9"/>
+        <v>293</v>
+      </c>
+      <c r="AB14" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC14" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD14" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE14" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH14" s="6">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="AI14" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ14" s="11">
+        <v>587</v>
+      </c>
+      <c r="AK14" s="11">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>G3</v>
+      </c>
+      <c r="N15" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>G6</v>
+      </c>
+      <c r="O15" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>A5</v>
+      </c>
+      <c r="P15" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>D4</v>
+      </c>
+      <c r="Q15" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>C5</v>
+      </c>
+      <c r="R15" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S15" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T15" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U15" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V15" s="17"/>
+      <c r="W15" s="10">
+        <f t="shared" si="11"/>
+        <v>196</v>
+      </c>
+      <c r="X15" s="10">
+        <f t="shared" si="9"/>
+        <v>1567</v>
+      </c>
+      <c r="Y15" s="10">
+        <f t="shared" si="9"/>
+        <v>880</v>
+      </c>
+      <c r="Z15" s="10">
+        <f t="shared" si="9"/>
+        <v>293</v>
+      </c>
+      <c r="AA15" s="10">
+        <f t="shared" si="9"/>
+        <v>523</v>
+      </c>
+      <c r="AB15" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC15" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD15" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE15" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH15" s="6">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="AI15" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ15" s="11">
+        <v>659</v>
+      </c>
+      <c r="AK15" s="11">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>E5</v>
+      </c>
+      <c r="N16" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="O16" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>G4</v>
+      </c>
+      <c r="P16" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q16" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R16" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S16" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T16" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U16" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V16" s="17"/>
+      <c r="W16" s="10">
+        <f t="shared" si="11"/>
+        <v>659</v>
+      </c>
+      <c r="X16" s="22">
+        <f t="shared" si="9"/>
+        <v>329</v>
+      </c>
+      <c r="Y16" s="10">
+        <f t="shared" si="9"/>
+        <v>392</v>
+      </c>
+      <c r="Z16" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA16" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB16" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC16" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD16" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE16" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH16" s="6">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="AI16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ16" s="11">
+        <v>784</v>
+      </c>
+      <c r="AK16" s="11">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A6</v>
+      </c>
+      <c r="N17" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>A3</v>
+      </c>
+      <c r="O17" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P17" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q17" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R17" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S17" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T17" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U17" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V17" s="17"/>
+      <c r="W17" s="10">
+        <f t="shared" si="11"/>
+        <v>1760</v>
+      </c>
+      <c r="X17" s="10">
+        <f t="shared" si="9"/>
+        <v>220</v>
+      </c>
+      <c r="Y17" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Z17" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA17" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB17" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC17" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD17" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE17" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH17" s="6">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="AI17" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ17" s="11">
+        <v>880</v>
+      </c>
+      <c r="AK17" s="11">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A6</v>
+      </c>
+      <c r="N18" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>C5</v>
+      </c>
+      <c r="O18" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P18" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q18" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R18" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S18" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T18" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U18" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V18" s="17"/>
+      <c r="W18" s="10">
+        <f t="shared" si="11"/>
+        <v>1760</v>
+      </c>
+      <c r="X18" s="10">
+        <f t="shared" si="9"/>
+        <v>523</v>
+      </c>
+      <c r="Y18" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Z18" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA18" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB18" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC18" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD18" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE18" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH18" s="6">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="AI18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ18" s="5">
+        <v>1046</v>
+      </c>
+      <c r="AK18" s="5">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>E5</v>
+      </c>
+      <c r="N19" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>D4</v>
+      </c>
+      <c r="O19" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>C4</v>
+      </c>
+      <c r="P19" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>E4</v>
+      </c>
+      <c r="Q19" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R19" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S19" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T19" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U19" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V19" s="17"/>
+      <c r="W19" s="10">
+        <f t="shared" si="11"/>
+        <v>659</v>
+      </c>
+      <c r="X19" s="10">
+        <f t="shared" si="9"/>
+        <v>293</v>
+      </c>
+      <c r="Y19" s="10">
+        <f t="shared" si="9"/>
+        <v>261</v>
+      </c>
+      <c r="Z19" s="10">
+        <f t="shared" si="9"/>
+        <v>329</v>
+      </c>
+      <c r="AA19" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB19" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC19" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD19" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE19" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH19" s="6">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="AI19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ19" s="5">
+        <v>1174</v>
+      </c>
+      <c r="AK19" s="5">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>A4</v>
+      </c>
+      <c r="N20" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>A6</v>
+      </c>
+      <c r="O20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P20" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q20" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R20" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S20" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T20" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="U20" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="V20" s="17"/>
+      <c r="W20" s="10">
+        <f t="shared" si="11"/>
+        <v>440</v>
+      </c>
+      <c r="X20" s="10">
+        <f t="shared" si="9"/>
+        <v>1760</v>
+      </c>
+      <c r="Y20" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Z20" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AA20" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AB20" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AC20" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AD20" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AE20" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="AG20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH20" s="6">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AI20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ20" s="5">
+        <v>1318</v>
+      </c>
+      <c r="AK20" s="5">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="10" t="str">
+        <f t="shared" ref="M21:U27" si="12">IFERROR(VLOOKUP(C21,$AG$5:$AI$30,3,FALSE), "")</f>
+        <v>G4</v>
+      </c>
+      <c r="N21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>G3</v>
+      </c>
+      <c r="O21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="P21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="Q21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="R21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="S21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="T21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="U21" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="V21" s="17"/>
+      <c r="W21" s="10">
+        <f t="shared" si="11"/>
+        <v>392</v>
+      </c>
+      <c r="X21" s="10">
+        <f t="shared" ref="X21:X27" si="13">IFERROR(VLOOKUP(D21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v>196</v>
+      </c>
+      <c r="Y21" s="10" t="str">
+        <f t="shared" ref="Y21:Y27" si="14">IFERROR(VLOOKUP(E21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="Z21" s="10" t="str">
+        <f t="shared" ref="Z21:Z27" si="15">IFERROR(VLOOKUP(F21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="AA21" s="10" t="str">
+        <f t="shared" ref="AA21:AA27" si="16">IFERROR(VLOOKUP(G21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="AB21" s="10" t="str">
+        <f t="shared" ref="AB21:AB27" si="17">IFERROR(VLOOKUP(H21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="AC21" s="10" t="str">
+        <f t="shared" ref="AC21:AC27" si="18">IFERROR(VLOOKUP(I21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="AD21" s="10" t="str">
+        <f t="shared" ref="AD21:AD27" si="19">IFERROR(VLOOKUP(J21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="AE21" s="10" t="str">
+        <f t="shared" ref="AE21:AE27" si="20">IFERROR(VLOOKUP(K21,$AG$5:$AJ$30,4,FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="AG21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH21" s="6">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AI21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ21" s="5">
+        <v>1567</v>
+      </c>
+      <c r="AK21" s="5">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>C4</v>
+      </c>
+      <c r="N22" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>E4</v>
+      </c>
+      <c r="O22" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>G5</v>
+      </c>
+      <c r="P22" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>A6</v>
+      </c>
+      <c r="Q22" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>A3</v>
+      </c>
+      <c r="R22" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>G3</v>
+      </c>
+      <c r="S22" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>A4</v>
+      </c>
+      <c r="T22" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="U22" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="V22" s="17"/>
+      <c r="W22" s="22">
+        <f t="shared" si="11"/>
+        <v>261</v>
+      </c>
+      <c r="X22" s="22">
+        <f t="shared" si="13"/>
+        <v>329</v>
+      </c>
+      <c r="Y22" s="10">
+        <f t="shared" si="14"/>
+        <v>784</v>
+      </c>
+      <c r="Z22" s="10">
+        <f t="shared" si="15"/>
+        <v>1760</v>
+      </c>
+      <c r="AA22" s="10">
+        <f t="shared" si="16"/>
+        <v>220</v>
+      </c>
+      <c r="AB22" s="10">
+        <f t="shared" si="17"/>
+        <v>196</v>
+      </c>
+      <c r="AC22" s="10">
+        <f t="shared" si="18"/>
+        <v>440</v>
+      </c>
+      <c r="AD22" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="AE22" s="10" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="AG22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH22" s="6">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AI22" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ22" s="11">
+        <v>174</v>
+      </c>
+      <c r="AK22" s="11">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>D6</v>
+      </c>
+      <c r="N23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>D4</v>
+      </c>
+      <c r="O23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="P23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="Q23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="R23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="S23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="T23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="U23" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="V23" s="17"/>
+      <c r="W23" s="10">
+        <f t="shared" si="11"/>
+        <v>1174</v>
+      </c>
+      <c r="X23" s="10">
+        <f t="shared" si="13"/>
+        <v>293</v>
+      </c>
+      <c r="Y23" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="Z23" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AA23" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AB23" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="AC23" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AD23" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="AE23" s="10" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="AG23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH23" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>F3</v>
+      </c>
+      <c r="N24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="O24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="P24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="Q24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="R24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="S24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="T24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="U24" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="V24" s="17"/>
+      <c r="W24" s="10">
+        <f t="shared" si="11"/>
+        <v>174</v>
+      </c>
+      <c r="X24" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y24" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="Z24" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AA24" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AB24" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="AC24" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AD24" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="AE24" s="10" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="AG24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH24" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>C4</v>
+      </c>
+      <c r="N25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>E4</v>
+      </c>
+      <c r="O25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>C5</v>
+      </c>
+      <c r="P25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="Q25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="R25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="S25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="T25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="U25" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="V25" s="17"/>
+      <c r="W25" s="10">
+        <f t="shared" si="11"/>
+        <v>261</v>
+      </c>
+      <c r="X25" s="10">
+        <f t="shared" si="13"/>
+        <v>329</v>
+      </c>
+      <c r="Y25" s="10">
+        <f t="shared" si="14"/>
+        <v>523</v>
+      </c>
+      <c r="Z25" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="AA25" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="AB25" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="AC25" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AD25" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="AE25" s="10" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="AG25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH25" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>A4</v>
+      </c>
+      <c r="N26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>E4</v>
+      </c>
+      <c r="O26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>C6</v>
+      </c>
+      <c r="P26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>C5</v>
+      </c>
+      <c r="Q26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>A6</v>
+      </c>
+      <c r="R26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="S26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="T26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="U26" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="V26" s="17"/>
+      <c r="W26" s="10">
+        <f t="shared" si="11"/>
+        <v>440</v>
+      </c>
+      <c r="X26" s="10">
+        <f t="shared" si="13"/>
+        <v>329</v>
+      </c>
+      <c r="Y26" s="10">
+        <f t="shared" si="14"/>
+        <v>1046</v>
+      </c>
+      <c r="Z26" s="10">
+        <f t="shared" si="15"/>
+        <v>523</v>
+      </c>
+      <c r="AA26" s="10">
+        <f t="shared" si="16"/>
+        <v>1760</v>
+      </c>
+      <c r="AB26" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="AC26" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AD26" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="AE26" s="10" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="AG26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH26" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>C6</v>
+      </c>
+      <c r="N27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>A6</v>
+      </c>
+      <c r="O27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>G4</v>
+      </c>
+      <c r="P27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>E4</v>
+      </c>
+      <c r="Q27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v>C5</v>
+      </c>
+      <c r="R27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="S27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="T27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="U27" s="10" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="V27" s="17"/>
+      <c r="W27" s="10">
+        <f t="shared" si="11"/>
+        <v>1046</v>
+      </c>
+      <c r="X27" s="10">
+        <f t="shared" si="13"/>
+        <v>1760</v>
+      </c>
+      <c r="Y27" s="10">
+        <f t="shared" si="14"/>
+        <v>392</v>
+      </c>
+      <c r="Z27" s="10">
+        <f t="shared" si="15"/>
+        <v>329</v>
+      </c>
+      <c r="AA27" s="10">
+        <f t="shared" si="16"/>
+        <v>523</v>
+      </c>
+      <c r="AB27" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="AC27" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="AD27" s="10" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="AE27" s="10" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="AG27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH27" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AG28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH28" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AG29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH29" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AG30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH30" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AG31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH31" s="4">
+        <f>COUNTIF(AH5:AH30, "&lt;&gt;0")</f>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AG4:AH4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="AG5:AG31">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>"IF($W$2:$W$27&lt;&gt;"""")"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH5:AH30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:bulb: test of the AI tool for audio isolation
</commit_message>
<xml_diff>
--- a/Cipher-key-music-text.xlsx
+++ b/Cipher-key-music-text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\OneDrive\Documentos\Signals Project\Fourier-Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745682F1-E4F9-42E8-8E66-483AC534762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35E9E1B-2461-47A8-8CAC-AB1D7163C5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{1D06FA13-21DA-4E25-B74A-0658B95FA3B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="99">
   <si>
     <t>En música, dos notas enarmónicas tienen diferente nombre pero suenan igual. Como en el caso de Mi sostenido, Fa, y Sol doble bemol</t>
   </si>
@@ -322,6 +322,18 @@
   </si>
   <si>
     <t>F3</t>
+  </si>
+  <si>
+    <t>paz</t>
+  </si>
+  <si>
+    <t>arbol</t>
+  </si>
+  <si>
+    <t>zote</t>
+  </si>
+  <si>
+    <t>pito</t>
   </si>
 </sst>
 </file>
@@ -443,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -470,15 +482,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -829,10 +839,10 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="W4" s="18" t="s">
+      <c r="W4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="X4" s="19"/>
+      <c r="X4" s="20"/>
       <c r="Y4" s="3" t="s">
         <v>93</v>
       </c>
@@ -853,10 +863,10 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="21">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -935,10 +945,10 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="21">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1025,10 +1035,10 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+      <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1109,10 +1119,10 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
+      <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1197,10 +1207,10 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
+      <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1284,10 +1294,10 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
+      <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1361,10 +1371,10 @@
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1444,10 +1454,10 @@
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
+      <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1525,10 +1535,10 @@
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
+      <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1602,10 +1612,10 @@
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
+      <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1681,10 +1691,10 @@
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
+      <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1760,10 +1770,10 @@
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" s="21">
+      <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1835,10 +1845,10 @@
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
+      <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1908,10 +1918,10 @@
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="21">
+      <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1981,10 +1991,10 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="21">
+      <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -2058,10 +2068,10 @@
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A20" s="21">
+      <c r="A20">
         <v>16</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -2131,10 +2141,10 @@
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A21" s="21">
+      <c r="A21">
         <v>17</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -2204,10 +2214,10 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A22" s="21">
+      <c r="A22">
         <v>18</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -2287,10 +2297,10 @@
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A23" s="21">
+      <c r="A23">
         <v>19</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -2351,10 +2361,10 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A24" s="21">
+      <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -2413,10 +2423,10 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A25" s="21">
+      <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -2479,10 +2489,10 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A26" s="21">
+      <c r="A26">
         <v>22</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -2549,10 +2559,10 @@
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A27" s="21">
+      <c r="A27">
         <v>23</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -2685,10 +2695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8CF093-7BA6-4B9D-9E3D-86BEDD90B65B}">
-  <dimension ref="A2:AP31"/>
+  <dimension ref="A2:AP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="95" workbookViewId="0">
+      <selection activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2706,10 +2716,10 @@
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="AG4" s="18" t="s">
+      <c r="AG4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="AH4" s="19"/>
+      <c r="AH4" s="20"/>
       <c r="AI4" s="3" t="s">
         <v>93</v>
       </c>
@@ -3264,11 +3274,11 @@
         <f t="shared" si="0"/>
         <v>A6</v>
       </c>
-      <c r="N9" s="22" t="str">
+      <c r="N9" s="18" t="str">
         <f t="shared" si="1"/>
         <v>A3</v>
       </c>
-      <c r="O9" s="22" t="str">
+      <c r="O9" s="18" t="str">
         <f t="shared" si="2"/>
         <v>D4</v>
       </c>
@@ -3301,11 +3311,11 @@
         <f t="shared" si="11"/>
         <v>1760</v>
       </c>
-      <c r="X9" s="22">
+      <c r="X9" s="18">
         <f t="shared" si="9"/>
         <v>220</v>
       </c>
-      <c r="Y9" s="22">
+      <c r="Y9" s="18">
         <f t="shared" si="9"/>
         <v>293</v>
       </c>
@@ -3383,11 +3393,11 @@
         <f t="shared" si="1"/>
         <v>G3</v>
       </c>
-      <c r="O10" s="22" t="str">
+      <c r="O10" s="18" t="str">
         <f t="shared" si="2"/>
         <v>A6</v>
       </c>
-      <c r="P10" s="22" t="str">
+      <c r="P10" s="18" t="str">
         <f t="shared" si="3"/>
         <v>A3</v>
       </c>
@@ -3420,11 +3430,11 @@
         <f t="shared" si="9"/>
         <v>196</v>
       </c>
-      <c r="Y10" s="22">
+      <c r="Y10" s="18">
         <f t="shared" si="9"/>
         <v>1760</v>
       </c>
-      <c r="Z10" s="22">
+      <c r="Z10" s="18">
         <f t="shared" si="9"/>
         <v>220</v>
       </c>
@@ -3508,7 +3518,7 @@
         <f t="shared" si="2"/>
         <v>D6</v>
       </c>
-      <c r="P11" s="22" t="str">
+      <c r="P11" s="18" t="str">
         <f t="shared" si="3"/>
         <v>A6</v>
       </c>
@@ -3545,7 +3555,7 @@
         <f t="shared" si="9"/>
         <v>1174</v>
       </c>
-      <c r="Z11" s="22">
+      <c r="Z11" s="18">
         <f t="shared" si="9"/>
         <v>1760</v>
       </c>
@@ -3859,7 +3869,7 @@
         <f t="shared" si="2"/>
         <v>A6</v>
       </c>
-      <c r="P14" s="22" t="str">
+      <c r="P14" s="18" t="str">
         <f t="shared" si="3"/>
         <v>A3</v>
       </c>
@@ -3896,7 +3906,7 @@
         <f t="shared" si="9"/>
         <v>1760</v>
       </c>
-      <c r="Z14" s="22">
+      <c r="Z14" s="18">
         <f t="shared" si="9"/>
         <v>220</v>
       </c>
@@ -4081,7 +4091,7 @@
         <f t="shared" si="0"/>
         <v>E5</v>
       </c>
-      <c r="N16" s="22" t="str">
+      <c r="N16" s="18" t="str">
         <f t="shared" si="1"/>
         <v>E4</v>
       </c>
@@ -4118,7 +4128,7 @@
         <f t="shared" si="11"/>
         <v>659</v>
       </c>
-      <c r="X16" s="22">
+      <c r="X16" s="18">
         <f t="shared" si="9"/>
         <v>329</v>
       </c>
@@ -4757,11 +4767,11 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="17"/>
-      <c r="M22" s="22" t="str">
+      <c r="M22" s="18" t="str">
         <f t="shared" si="12"/>
         <v>C4</v>
       </c>
-      <c r="N22" s="22" t="str">
+      <c r="N22" s="18" t="str">
         <f t="shared" si="12"/>
         <v>E4</v>
       </c>
@@ -4794,11 +4804,11 @@
         <v/>
       </c>
       <c r="V22" s="17"/>
-      <c r="W22" s="22">
+      <c r="W22" s="18">
         <f t="shared" si="11"/>
         <v>261</v>
       </c>
-      <c r="X22" s="22">
+      <c r="X22" s="18">
         <f t="shared" si="13"/>
         <v>329</v>
       </c>
@@ -5397,12 +5407,30 @@
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="V31" t="s">
+        <v>95</v>
+      </c>
       <c r="AG31" s="4" t="s">
         <v>68</v>
       </c>
       <c r="AH31" s="4">
         <f>COUNTIF(AH5:AH30, "&lt;&gt;0")</f>
         <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="V32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="22:22" x14ac:dyDescent="0.3">
+      <c r="V33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="22:22" x14ac:dyDescent="0.3">
+      <c r="V34" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>